<commit_message>
refs #658 5xL ergänzt
</commit_message>
<xml_diff>
--- a/doc/Bericht/05_Technischer Bericht/03_Vorstudie/Frageboegen_Statistik.xlsx
+++ b/doc/Bericht/05_Technischer Bericht/03_Vorstudie/Frageboegen_Statistik.xlsx
@@ -572,28 +572,28 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>2.6111111111111112</c:v>
+                  <c:v>2.7826086956521738</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.6111111111111112</c:v>
+                  <c:v>1.7391304347826086</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3</c:v>
+                  <c:v>3.0952380952380953</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2</c:v>
+                  <c:v>2.1304347826086958</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2.8823529411764706</c:v>
+                  <c:v>3.0454545454545454</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>2.2222222222222223</c:v>
+                  <c:v>2.2272727272727271</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1.8888888888888888</c:v>
+                  <c:v>1.826086956521739</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>2.7222222222222223</c:v>
+                  <c:v>2.6086956521739131</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1014,11 +1014,11 @@
         </c:dLbls>
         <c:gapWidth val="75"/>
         <c:overlap val="-25"/>
-        <c:axId val="107421696"/>
-        <c:axId val="107423232"/>
+        <c:axId val="78983168"/>
+        <c:axId val="78984704"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="107421696"/>
+        <c:axId val="78983168"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -1028,7 +1028,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="107423232"/>
+        <c:crossAx val="78984704"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1037,7 +1037,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="107423232"/>
+        <c:axId val="78984704"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="4"/>
@@ -1100,7 +1100,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="107421696"/>
+        <c:crossAx val="78983168"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="1"/>
@@ -1154,7 +1154,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -1255,11 +1254,11 @@
         </c:dLbls>
         <c:gapWidth val="75"/>
         <c:overlap val="-25"/>
-        <c:axId val="109329408"/>
-        <c:axId val="109335296"/>
+        <c:axId val="81669120"/>
+        <c:axId val="81675008"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="109329408"/>
+        <c:axId val="81669120"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -1269,7 +1268,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="109335296"/>
+        <c:crossAx val="81675008"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1278,7 +1277,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="109335296"/>
+        <c:axId val="81675008"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="4"/>
@@ -1341,7 +1340,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="109329408"/>
+        <c:crossAx val="81669120"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="1"/>
@@ -1350,7 +1349,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -1400,7 +1398,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -1744,11 +1741,11 @@
         </c:dLbls>
         <c:gapWidth val="75"/>
         <c:overlap val="-25"/>
-        <c:axId val="109400064"/>
-        <c:axId val="109401600"/>
+        <c:axId val="81747968"/>
+        <c:axId val="81749504"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="109400064"/>
+        <c:axId val="81747968"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -1758,7 +1755,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="109401600"/>
+        <c:crossAx val="81749504"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1767,7 +1764,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="109401600"/>
+        <c:axId val="81749504"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="4"/>
@@ -1830,7 +1827,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="109400064"/>
+        <c:crossAx val="81747968"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="1"/>
@@ -1839,7 +1836,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -1884,7 +1880,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -1985,11 +1980,11 @@
         </c:dLbls>
         <c:gapWidth val="75"/>
         <c:overlap val="-25"/>
-        <c:axId val="109430656"/>
-        <c:axId val="109432192"/>
+        <c:axId val="81774464"/>
+        <c:axId val="81776000"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="109430656"/>
+        <c:axId val="81774464"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -1999,7 +1994,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="109432192"/>
+        <c:crossAx val="81776000"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2008,7 +2003,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="109432192"/>
+        <c:axId val="81776000"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="4"/>
@@ -2071,7 +2066,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="109430656"/>
+        <c:crossAx val="81774464"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="1"/>
@@ -2080,7 +2075,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -2159,7 +2153,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -2422,11 +2415,11 @@
         </c:dLbls>
         <c:gapWidth val="75"/>
         <c:overlap val="-25"/>
-        <c:axId val="111806336"/>
-        <c:axId val="111807872"/>
+        <c:axId val="96733056"/>
+        <c:axId val="96734592"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="111806336"/>
+        <c:axId val="96733056"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -2436,7 +2429,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="111807872"/>
+        <c:crossAx val="96734592"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2445,7 +2438,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="111807872"/>
+        <c:axId val="96734592"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="4"/>
@@ -2508,7 +2501,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="111806336"/>
+        <c:crossAx val="96733056"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="1"/>
@@ -2517,7 +2510,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -2567,7 +2559,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -2668,11 +2659,11 @@
         </c:dLbls>
         <c:gapWidth val="75"/>
         <c:overlap val="-25"/>
-        <c:axId val="111853568"/>
-        <c:axId val="111855104"/>
+        <c:axId val="96784384"/>
+        <c:axId val="96785920"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="111853568"/>
+        <c:axId val="96784384"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -2682,7 +2673,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="111855104"/>
+        <c:crossAx val="96785920"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2691,7 +2682,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="111855104"/>
+        <c:axId val="96785920"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="4"/>
@@ -2754,7 +2745,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="111853568"/>
+        <c:crossAx val="96784384"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="1"/>
@@ -2763,7 +2754,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -2819,7 +2809,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -3067,11 +3056,11 @@
         </c:dLbls>
         <c:gapWidth val="75"/>
         <c:overlap val="-25"/>
-        <c:axId val="116626176"/>
-        <c:axId val="116627712"/>
+        <c:axId val="97878784"/>
+        <c:axId val="97880320"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="116626176"/>
+        <c:axId val="97878784"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -3081,7 +3070,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="116627712"/>
+        <c:crossAx val="97880320"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3090,7 +3079,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="116627712"/>
+        <c:axId val="97880320"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="4"/>
@@ -3153,7 +3142,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="116626176"/>
+        <c:crossAx val="97878784"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="1"/>
@@ -3162,7 +3151,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -3207,7 +3195,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -3308,11 +3295,11 @@
         </c:dLbls>
         <c:gapWidth val="75"/>
         <c:overlap val="-25"/>
-        <c:axId val="116652672"/>
-        <c:axId val="116330880"/>
+        <c:axId val="97909376"/>
+        <c:axId val="97980800"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="116652672"/>
+        <c:axId val="97909376"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -3322,7 +3309,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="116330880"/>
+        <c:crossAx val="97980800"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3331,7 +3318,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="116330880"/>
+        <c:axId val="97980800"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="4"/>
@@ -3394,7 +3381,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="116652672"/>
+        <c:crossAx val="97909376"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="1"/>
@@ -3403,7 +3390,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -3544,28 +3530,28 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>2.3969849246231156</c:v>
+                  <c:v>2.4215686274509802</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.8442211055276383</c:v>
+                  <c:v>1.8529411764705883</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2.9057591623036649</c:v>
+                  <c:v>2.9175257731958761</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2.3883248730964466</c:v>
+                  <c:v>2.3935643564356437</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2.7268041237113403</c:v>
+                  <c:v>2.7487437185929648</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>2.6269035532994924</c:v>
+                  <c:v>2.6194029850746268</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1.9441624365482233</c:v>
+                  <c:v>1.9356435643564356</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>3.0351758793969847</c:v>
+                  <c:v>3.0147058823529411</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3581,11 +3567,11 @@
         </c:dLbls>
         <c:gapWidth val="75"/>
         <c:overlap val="-25"/>
-        <c:axId val="107448576"/>
-        <c:axId val="107470848"/>
+        <c:axId val="79010048"/>
+        <c:axId val="79032320"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="107448576"/>
+        <c:axId val="79010048"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -3595,7 +3581,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="107470848"/>
+        <c:crossAx val="79032320"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3604,7 +3590,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="107470848"/>
+        <c:axId val="79032320"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="4"/>
@@ -3667,7 +3653,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="107448576"/>
+        <c:crossAx val="79010048"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="1"/>
@@ -3750,7 +3736,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -4013,11 +3998,11 @@
         </c:dLbls>
         <c:gapWidth val="75"/>
         <c:overlap val="-25"/>
-        <c:axId val="107521920"/>
-        <c:axId val="107523456"/>
+        <c:axId val="79792000"/>
+        <c:axId val="79793536"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="107521920"/>
+        <c:axId val="79792000"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -4027,7 +4012,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="107523456"/>
+        <c:crossAx val="79793536"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4036,7 +4021,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="107523456"/>
+        <c:axId val="79793536"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="4"/>
@@ -4099,7 +4084,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="107521920"/>
+        <c:crossAx val="79792000"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="1"/>
@@ -4108,7 +4093,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -4153,7 +4137,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -4254,11 +4237,11 @@
         </c:dLbls>
         <c:gapWidth val="75"/>
         <c:overlap val="-25"/>
-        <c:axId val="109192704"/>
-        <c:axId val="109194240"/>
+        <c:axId val="81539072"/>
+        <c:axId val="81540608"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="109192704"/>
+        <c:axId val="81539072"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -4268,7 +4251,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="109194240"/>
+        <c:crossAx val="81540608"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4277,7 +4260,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="109194240"/>
+        <c:axId val="81540608"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="4"/>
@@ -4340,7 +4323,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="109192704"/>
+        <c:crossAx val="81539072"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="1"/>
@@ -4349,7 +4332,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -4492,28 +4474,28 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>2.6111111111111112</c:v>
+                  <c:v>2.7826086956521738</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.6111111111111112</c:v>
+                  <c:v>1.7391304347826086</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3</c:v>
+                  <c:v>3.0952380952380953</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2</c:v>
+                  <c:v>2.1304347826086958</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2.8823529411764706</c:v>
+                  <c:v>3.0454545454545454</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>2.2222222222222223</c:v>
+                  <c:v>2.2272727272727271</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1.8888888888888888</c:v>
+                  <c:v>1.826086956521739</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>2.7222222222222223</c:v>
+                  <c:v>2.6086956521739131</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4654,28 +4636,28 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>4</c:v>
+                  <c:v>3.5</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>4</c:v>
+                  <c:v>3.75</c:v>
                 </c:pt>
                 <c:pt idx="3">
+                  <c:v>2.5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3.5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2.2000000000000002</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.6666666666666667</c:v>
+                </c:pt>
+                <c:pt idx="7">
                   <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>1</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4772,11 +4754,11 @@
         </c:dLbls>
         <c:gapWidth val="75"/>
         <c:overlap val="-25"/>
-        <c:axId val="109263488"/>
-        <c:axId val="109277568"/>
+        <c:axId val="81607296"/>
+        <c:axId val="81617280"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="109263488"/>
+        <c:axId val="81607296"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -4786,7 +4768,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="109277568"/>
+        <c:crossAx val="81617280"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4795,7 +4777,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="109277568"/>
+        <c:axId val="81617280"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="4"/>
@@ -4858,7 +4840,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="109263488"/>
+        <c:crossAx val="81607296"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="1"/>
@@ -4976,28 +4958,28 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>2.6111111111111112</c:v>
+                  <c:v>2.7826086956521738</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.6111111111111112</c:v>
+                  <c:v>1.7391304347826086</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3</c:v>
+                  <c:v>3.0952380952380953</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2</c:v>
+                  <c:v>2.1304347826086958</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2.8823529411764706</c:v>
+                  <c:v>3.0454545454545454</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>2.2222222222222223</c:v>
+                  <c:v>2.2272727272727271</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1.8888888888888888</c:v>
+                  <c:v>1.826086956521739</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>2.7222222222222223</c:v>
+                  <c:v>2.6086956521739131</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5013,11 +4995,11 @@
         </c:dLbls>
         <c:gapWidth val="75"/>
         <c:overlap val="-25"/>
-        <c:axId val="109302528"/>
-        <c:axId val="109304064"/>
+        <c:axId val="81631872"/>
+        <c:axId val="81650048"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="109302528"/>
+        <c:axId val="81631872"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -5027,7 +5009,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="109304064"/>
+        <c:crossAx val="81650048"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -5036,7 +5018,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="109304064"/>
+        <c:axId val="81650048"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="4"/>
@@ -5099,7 +5081,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="109302528"/>
+        <c:crossAx val="81631872"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="1"/>
@@ -5187,7 +5169,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -5450,11 +5431,11 @@
         </c:dLbls>
         <c:gapWidth val="75"/>
         <c:overlap val="-25"/>
-        <c:axId val="108972672"/>
-        <c:axId val="108974464"/>
+        <c:axId val="81316096"/>
+        <c:axId val="81321984"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="108972672"/>
+        <c:axId val="81316096"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -5464,7 +5445,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="108974464"/>
+        <c:crossAx val="81321984"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -5473,7 +5454,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="108974464"/>
+        <c:axId val="81321984"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="4"/>
@@ -5536,7 +5517,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="108972672"/>
+        <c:crossAx val="81316096"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="1"/>
@@ -5545,7 +5526,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -5590,7 +5570,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -5691,11 +5670,11 @@
         </c:dLbls>
         <c:gapWidth val="75"/>
         <c:overlap val="-25"/>
-        <c:axId val="109003136"/>
-        <c:axId val="109004672"/>
+        <c:axId val="81351040"/>
+        <c:axId val="81352576"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="109003136"/>
+        <c:axId val="81351040"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -5705,7 +5684,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="109004672"/>
+        <c:crossAx val="81352576"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -5714,7 +5693,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="109004672"/>
+        <c:axId val="81352576"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="4"/>
@@ -5777,7 +5756,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="109003136"/>
+        <c:crossAx val="81351040"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="1"/>
@@ -5786,7 +5765,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -5836,7 +5814,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -6180,11 +6157,11 @@
         </c:dLbls>
         <c:gapWidth val="75"/>
         <c:overlap val="-25"/>
-        <c:axId val="109155456"/>
-        <c:axId val="109156992"/>
+        <c:axId val="81499264"/>
+        <c:axId val="81500800"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="109155456"/>
+        <c:axId val="81499264"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -6194,7 +6171,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="109156992"/>
+        <c:crossAx val="81500800"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -6203,7 +6180,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="109156992"/>
+        <c:axId val="81500800"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="4"/>
@@ -6266,7 +6243,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="109155456"/>
+        <c:crossAx val="81499264"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="1"/>
@@ -6275,7 +6252,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -7132,7 +7108,7 @@
   <dimension ref="A1:Y32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J11" sqref="J11"/>
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7247,7 +7223,7 @@
         <v>1</v>
       </c>
       <c r="H4">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="J4" t="s">
         <v>1</v>
@@ -7315,7 +7291,7 @@
       </c>
       <c r="B6" s="16">
         <f>SUM(W6,E6,H6,K6,N6,Q6,T6)</f>
-        <v>199</v>
+        <v>204</v>
       </c>
       <c r="C6" s="6"/>
       <c r="D6" s="6" t="s">
@@ -7331,7 +7307,7 @@
       </c>
       <c r="H6" s="9">
         <f>SUM(H3:H5)</f>
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="I6" s="6"/>
       <c r="J6" s="6" t="s">
@@ -7412,7 +7388,7 @@
       </c>
       <c r="G10">
         <f>Landschaftsarchitektur!Q4</f>
-        <v>47</v>
+        <v>64</v>
       </c>
       <c r="J10">
         <f>Raumplanung!M4</f>
@@ -7436,11 +7412,11 @@
       </c>
       <c r="X10">
         <f>Bauingenieurwesen!X4+Landschaftsarchitektur!R4+Raumplanung!N4+Elektrotechnik!P4+Maschinentechnik!Z4+EEU!R4+Informatik!X4</f>
-        <v>199</v>
+        <v>204</v>
       </c>
       <c r="Y10" s="12">
         <f>(D10+G10+J10+M10+P10+S10+V10)/X10</f>
-        <v>2.3969849246231156</v>
+        <v>2.4215686274509802</v>
       </c>
     </row>
     <row r="11" spans="1:25" x14ac:dyDescent="0.25">
@@ -7453,7 +7429,7 @@
       </c>
       <c r="G11">
         <f>Landschaftsarchitektur!Q5</f>
-        <v>29</v>
+        <v>40</v>
       </c>
       <c r="J11">
         <f>Raumplanung!M5</f>
@@ -7477,11 +7453,11 @@
       </c>
       <c r="X11">
         <f>Bauingenieurwesen!X5+Landschaftsarchitektur!R5+Raumplanung!N5+Elektrotechnik!P5+Maschinentechnik!Z5+EEU!R5+Informatik!X5</f>
-        <v>199</v>
+        <v>204</v>
       </c>
       <c r="Y11" s="12">
         <f t="shared" ref="Y11:Y17" si="0">(D11+G11+J11+M11+P11+S11+V11)/X11</f>
-        <v>1.8442211055276383</v>
+        <v>1.8529411764705883</v>
       </c>
     </row>
     <row r="12" spans="1:25" x14ac:dyDescent="0.25">
@@ -7494,7 +7470,7 @@
       </c>
       <c r="G12">
         <f>Landschaftsarchitektur!Q6</f>
-        <v>54</v>
+        <v>65</v>
       </c>
       <c r="J12">
         <f>Raumplanung!M6</f>
@@ -7518,11 +7494,11 @@
       </c>
       <c r="X12">
         <f>Bauingenieurwesen!X6+Landschaftsarchitektur!R6+Raumplanung!N6+Elektrotechnik!P6+Maschinentechnik!Z6+EEU!R6+Informatik!X6</f>
-        <v>191</v>
+        <v>194</v>
       </c>
       <c r="Y12" s="12">
         <f t="shared" si="0"/>
-        <v>2.9057591623036649</v>
+        <v>2.9175257731958761</v>
       </c>
     </row>
     <row r="13" spans="1:25" x14ac:dyDescent="0.25">
@@ -7535,7 +7511,7 @@
       </c>
       <c r="G13">
         <f>Landschaftsarchitektur!Q7</f>
-        <v>36</v>
+        <v>49</v>
       </c>
       <c r="J13">
         <f>Raumplanung!M7</f>
@@ -7559,11 +7535,11 @@
       </c>
       <c r="X13">
         <f>Bauingenieurwesen!X7+Landschaftsarchitektur!R7+Raumplanung!N7+Elektrotechnik!P7+Maschinentechnik!Z7+EEU!R7+Informatik!X7</f>
-        <v>197</v>
+        <v>202</v>
       </c>
       <c r="Y13" s="12">
         <f t="shared" si="0"/>
-        <v>2.3883248730964466</v>
+        <v>2.3935643564356437</v>
       </c>
     </row>
     <row r="14" spans="1:25" x14ac:dyDescent="0.25">
@@ -7576,7 +7552,7 @@
       </c>
       <c r="G14">
         <f>Landschaftsarchitektur!Q8</f>
-        <v>49</v>
+        <v>67</v>
       </c>
       <c r="J14">
         <f>Raumplanung!M8</f>
@@ -7600,11 +7576,11 @@
       </c>
       <c r="X14">
         <f>Bauingenieurwesen!X8+Landschaftsarchitektur!R8+Raumplanung!N8+Elektrotechnik!P8+Maschinentechnik!Z8+EEU!R8+Informatik!X8</f>
-        <v>194</v>
+        <v>199</v>
       </c>
       <c r="Y14" s="12">
         <f t="shared" si="0"/>
-        <v>2.7268041237113403</v>
+        <v>2.7487437185929648</v>
       </c>
     </row>
     <row r="15" spans="1:25" x14ac:dyDescent="0.25">
@@ -7617,7 +7593,7 @@
       </c>
       <c r="G15">
         <f>Landschaftsarchitektur!Q9</f>
-        <v>40</v>
+        <v>49</v>
       </c>
       <c r="J15">
         <f>Raumplanung!M9</f>
@@ -7641,11 +7617,11 @@
       </c>
       <c r="X15">
         <f>Bauingenieurwesen!X9+Landschaftsarchitektur!R9+Raumplanung!N9+Elektrotechnik!P9+Maschinentechnik!Z9+EEU!R9+Informatik!X9</f>
-        <v>197</v>
+        <v>201</v>
       </c>
       <c r="Y15" s="12">
         <f t="shared" si="0"/>
-        <v>2.6269035532994924</v>
+        <v>2.6194029850746268</v>
       </c>
     </row>
     <row r="16" spans="1:25" x14ac:dyDescent="0.25">
@@ -7658,7 +7634,7 @@
       </c>
       <c r="G16">
         <f>Landschaftsarchitektur!Q10</f>
-        <v>34</v>
+        <v>42</v>
       </c>
       <c r="J16">
         <f>Raumplanung!M10</f>
@@ -7682,11 +7658,11 @@
       </c>
       <c r="X16">
         <f>Bauingenieurwesen!X10+Landschaftsarchitektur!R10+Raumplanung!N10+Elektrotechnik!P10+Maschinentechnik!Z10+EEU!R10+Informatik!X10</f>
-        <v>197</v>
+        <v>202</v>
       </c>
       <c r="Y16" s="12">
         <f t="shared" si="0"/>
-        <v>1.9441624365482233</v>
+        <v>1.9356435643564356</v>
       </c>
     </row>
     <row r="17" spans="1:25" x14ac:dyDescent="0.25">
@@ -7699,7 +7675,7 @@
       </c>
       <c r="G17">
         <f>Landschaftsarchitektur!Q11</f>
-        <v>49</v>
+        <v>60</v>
       </c>
       <c r="J17">
         <f>Raumplanung!M11</f>
@@ -7723,11 +7699,11 @@
       </c>
       <c r="X17">
         <f>Bauingenieurwesen!X11+Landschaftsarchitektur!R11+Raumplanung!N11+Elektrotechnik!P11+Maschinentechnik!Z11+EEU!R11+Informatik!X11</f>
-        <v>199</v>
+        <v>204</v>
       </c>
       <c r="Y17" s="13">
         <f t="shared" si="0"/>
-        <v>3.0351758793969847</v>
+        <v>3.0147058823529411</v>
       </c>
     </row>
     <row r="18" spans="1:25" x14ac:dyDescent="0.25">
@@ -9164,7 +9140,7 @@
   <dimension ref="A1:S43"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="AF18" sqref="AF18"/>
+      <selection activeCell="G34" sqref="G34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9191,7 +9167,7 @@
       <c r="G1" s="6"/>
       <c r="H1" s="9">
         <f>'Alle Abteilungen'!H6</f>
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="I1" s="6"/>
       <c r="J1" s="6"/>
@@ -9240,7 +9216,7 @@
       </c>
       <c r="C4">
         <f>Q26</f>
-        <v>4</v>
+        <v>21</v>
       </c>
       <c r="D4">
         <f>Q36</f>
@@ -9248,15 +9224,15 @@
       </c>
       <c r="Q4">
         <f>SUM(B4:P4)</f>
-        <v>47</v>
+        <v>64</v>
       </c>
       <c r="R4">
         <f t="shared" ref="R4:R11" si="0">R15+R26+R36</f>
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="S4" s="11">
         <f>Q4/R4</f>
-        <v>2.6111111111111112</v>
+        <v>2.7826086956521738</v>
       </c>
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.25">
@@ -9270,7 +9246,7 @@
       </c>
       <c r="C5">
         <f t="shared" ref="C5:C11" si="2">Q27</f>
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="D5">
         <f t="shared" ref="D5:D11" si="3">Q37</f>
@@ -9278,15 +9254,15 @@
       </c>
       <c r="Q5">
         <f t="shared" ref="Q5:Q11" si="4">SUM(B5:P5)</f>
-        <v>29</v>
+        <v>40</v>
       </c>
       <c r="R5">
         <f t="shared" si="0"/>
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="S5" s="12">
         <f t="shared" ref="S5:S11" si="5">Q5/R5</f>
-        <v>1.6111111111111112</v>
+        <v>1.7391304347826086</v>
       </c>
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.25">
@@ -9300,7 +9276,7 @@
       </c>
       <c r="C6">
         <f t="shared" si="2"/>
-        <v>4</v>
+        <v>15</v>
       </c>
       <c r="D6">
         <f t="shared" si="3"/>
@@ -9308,15 +9284,15 @@
       </c>
       <c r="Q6">
         <f t="shared" si="4"/>
-        <v>54</v>
+        <v>65</v>
       </c>
       <c r="R6">
         <f t="shared" si="0"/>
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="S6" s="12">
         <f t="shared" si="5"/>
-        <v>3</v>
+        <v>3.0952380952380953</v>
       </c>
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.25">
@@ -9330,7 +9306,7 @@
       </c>
       <c r="C7">
         <f t="shared" si="2"/>
-        <v>2</v>
+        <v>15</v>
       </c>
       <c r="D7">
         <f t="shared" si="3"/>
@@ -9338,15 +9314,15 @@
       </c>
       <c r="Q7">
         <f t="shared" si="4"/>
-        <v>36</v>
+        <v>49</v>
       </c>
       <c r="R7">
         <f t="shared" si="0"/>
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="S7" s="12">
         <f t="shared" si="5"/>
-        <v>2</v>
+        <v>2.1304347826086958</v>
       </c>
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.25">
@@ -9360,7 +9336,7 @@
       </c>
       <c r="C8">
         <f t="shared" si="2"/>
-        <v>3</v>
+        <v>21</v>
       </c>
       <c r="D8">
         <f t="shared" si="3"/>
@@ -9368,15 +9344,15 @@
       </c>
       <c r="Q8">
         <f t="shared" si="4"/>
-        <v>49</v>
+        <v>67</v>
       </c>
       <c r="R8">
         <f t="shared" si="0"/>
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="S8" s="12">
         <f t="shared" si="5"/>
-        <v>2.8823529411764706</v>
+        <v>3.0454545454545454</v>
       </c>
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.25">
@@ -9390,7 +9366,7 @@
       </c>
       <c r="C9">
         <f t="shared" si="2"/>
-        <v>2</v>
+        <v>11</v>
       </c>
       <c r="D9">
         <f t="shared" si="3"/>
@@ -9398,15 +9374,15 @@
       </c>
       <c r="Q9">
         <f t="shared" si="4"/>
-        <v>40</v>
+        <v>49</v>
       </c>
       <c r="R9">
         <f t="shared" si="0"/>
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="S9" s="12">
         <f t="shared" si="5"/>
-        <v>2.2222222222222223</v>
+        <v>2.2272727272727271</v>
       </c>
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.25">
@@ -9420,7 +9396,7 @@
       </c>
       <c r="C10">
         <f t="shared" si="2"/>
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="D10">
         <f t="shared" si="3"/>
@@ -9428,15 +9404,15 @@
       </c>
       <c r="Q10">
         <f t="shared" si="4"/>
-        <v>34</v>
+        <v>42</v>
       </c>
       <c r="R10">
         <f t="shared" si="0"/>
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="S10" s="12">
         <f t="shared" si="5"/>
-        <v>1.8888888888888888</v>
+        <v>1.826086956521739</v>
       </c>
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.25">
@@ -9450,7 +9426,7 @@
       </c>
       <c r="C11">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="D11">
         <f t="shared" si="3"/>
@@ -9458,15 +9434,15 @@
       </c>
       <c r="Q11">
         <f t="shared" si="4"/>
-        <v>49</v>
+        <v>60</v>
       </c>
       <c r="R11">
         <f t="shared" si="0"/>
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="S11" s="13">
         <f t="shared" si="5"/>
-        <v>2.7222222222222223</v>
+        <v>2.6086956521739131</v>
       </c>
     </row>
     <row r="12" spans="1:19" x14ac:dyDescent="0.25">
@@ -10096,7 +10072,7 @@
       </c>
       <c r="B25" s="9">
         <f>'Alle Abteilungen'!H4</f>
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="C25" s="6" t="s">
         <v>18</v>
@@ -10128,17 +10104,32 @@
       <c r="B26">
         <v>4</v>
       </c>
+      <c r="C26">
+        <v>3</v>
+      </c>
+      <c r="D26">
+        <v>4</v>
+      </c>
+      <c r="E26">
+        <v>4</v>
+      </c>
+      <c r="F26">
+        <v>3</v>
+      </c>
+      <c r="G26">
+        <v>3</v>
+      </c>
       <c r="Q26">
         <f>SUM(B26:P26)</f>
-        <v>4</v>
+        <v>21</v>
       </c>
       <c r="R26">
         <f t="shared" ref="R26:R33" si="9">$B$25-SUMIF(B26:P26,0,$B$23:$P$23)</f>
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="S26" s="8">
         <f>Q26/R26</f>
-        <v>4</v>
+        <v>3.5</v>
       </c>
     </row>
     <row r="27" spans="1:19" x14ac:dyDescent="0.25">
@@ -10149,17 +10140,32 @@
       <c r="B27">
         <v>1</v>
       </c>
+      <c r="C27">
+        <v>2</v>
+      </c>
+      <c r="D27">
+        <v>2</v>
+      </c>
+      <c r="E27">
+        <v>4</v>
+      </c>
+      <c r="F27">
+        <v>2</v>
+      </c>
+      <c r="G27">
+        <v>1</v>
+      </c>
       <c r="Q27">
         <f t="shared" ref="Q27:Q33" si="10">SUM(B27:P27)</f>
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="R27">
         <f t="shared" si="9"/>
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="S27" s="8">
         <f t="shared" ref="S27:S33" si="11">Q27/R27</f>
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="28" spans="1:19" x14ac:dyDescent="0.25">
@@ -10170,17 +10176,32 @@
       <c r="B28">
         <v>4</v>
       </c>
+      <c r="C28">
+        <v>4</v>
+      </c>
+      <c r="D28">
+        <v>0</v>
+      </c>
+      <c r="E28">
+        <v>4</v>
+      </c>
+      <c r="F28">
+        <v>0</v>
+      </c>
+      <c r="G28">
+        <v>3</v>
+      </c>
       <c r="Q28">
         <f t="shared" si="10"/>
-        <v>4</v>
+        <v>15</v>
       </c>
       <c r="R28">
         <f t="shared" si="9"/>
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="S28" s="8">
         <f t="shared" si="11"/>
-        <v>4</v>
+        <v>3.75</v>
       </c>
     </row>
     <row r="29" spans="1:19" x14ac:dyDescent="0.25">
@@ -10191,17 +10212,32 @@
       <c r="B29">
         <v>2</v>
       </c>
+      <c r="C29">
+        <v>2</v>
+      </c>
+      <c r="D29">
+        <v>3</v>
+      </c>
+      <c r="E29">
+        <v>3</v>
+      </c>
+      <c r="F29">
+        <v>4</v>
+      </c>
+      <c r="G29">
+        <v>1</v>
+      </c>
       <c r="Q29">
         <f t="shared" si="10"/>
-        <v>2</v>
+        <v>15</v>
       </c>
       <c r="R29">
         <f t="shared" si="9"/>
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="S29" s="8">
         <f t="shared" si="11"/>
-        <v>2</v>
+        <v>2.5</v>
       </c>
     </row>
     <row r="30" spans="1:19" x14ac:dyDescent="0.25">
@@ -10212,17 +10248,32 @@
       <c r="B30">
         <v>3</v>
       </c>
+      <c r="C30">
+        <v>3</v>
+      </c>
+      <c r="D30">
+        <v>4</v>
+      </c>
+      <c r="E30">
+        <v>3</v>
+      </c>
+      <c r="F30">
+        <v>4</v>
+      </c>
+      <c r="G30">
+        <v>4</v>
+      </c>
       <c r="Q30">
         <f t="shared" si="10"/>
-        <v>3</v>
+        <v>21</v>
       </c>
       <c r="R30">
         <f t="shared" si="9"/>
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="S30" s="8">
         <f t="shared" si="11"/>
-        <v>3</v>
+        <v>3.5</v>
       </c>
     </row>
     <row r="31" spans="1:19" x14ac:dyDescent="0.25">
@@ -10233,17 +10284,32 @@
       <c r="B31">
         <v>2</v>
       </c>
+      <c r="C31">
+        <v>3</v>
+      </c>
+      <c r="D31">
+        <v>0</v>
+      </c>
+      <c r="E31">
+        <v>3</v>
+      </c>
+      <c r="F31">
+        <v>2</v>
+      </c>
+      <c r="G31">
+        <v>1</v>
+      </c>
       <c r="Q31">
         <f t="shared" si="10"/>
-        <v>2</v>
+        <v>11</v>
       </c>
       <c r="R31">
         <f t="shared" si="9"/>
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="S31" s="8">
         <f t="shared" si="11"/>
-        <v>2</v>
+        <v>2.2000000000000002</v>
       </c>
     </row>
     <row r="32" spans="1:19" x14ac:dyDescent="0.25">
@@ -10254,17 +10320,32 @@
       <c r="B32">
         <v>2</v>
       </c>
+      <c r="C32">
+        <v>2</v>
+      </c>
+      <c r="D32">
+        <v>2</v>
+      </c>
+      <c r="E32">
+        <v>2</v>
+      </c>
+      <c r="F32">
+        <v>1</v>
+      </c>
+      <c r="G32">
+        <v>1</v>
+      </c>
       <c r="Q32">
         <f t="shared" si="10"/>
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="R32">
         <f t="shared" si="9"/>
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="S32" s="8">
         <f t="shared" si="11"/>
-        <v>2</v>
+        <v>1.6666666666666667</v>
       </c>
     </row>
     <row r="33" spans="1:19" x14ac:dyDescent="0.25">
@@ -10275,17 +10356,32 @@
       <c r="B33">
         <v>1</v>
       </c>
+      <c r="C33">
+        <v>3</v>
+      </c>
+      <c r="D33">
+        <v>2</v>
+      </c>
+      <c r="E33">
+        <v>3</v>
+      </c>
+      <c r="F33">
+        <v>1</v>
+      </c>
+      <c r="G33">
+        <v>2</v>
+      </c>
       <c r="Q33">
         <f t="shared" si="10"/>
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="R33">
         <f t="shared" si="9"/>
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="S33" s="8">
         <f t="shared" si="11"/>
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="34" spans="1:19" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
refs #778 Anpassung an Vorstudie.docx
Former-commit-id: 621f68938443262a74179c3b8b2d225c159a6e6c
</commit_message>
<xml_diff>
--- a/doc/Bericht/05_Technischer Bericht/03_Vorstudie/Frageboegen_Statistik.xlsx
+++ b/doc/Bericht/05_Technischer Bericht/03_Vorstudie/Frageboegen_Statistik.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="120" windowWidth="20835" windowHeight="12015" tabRatio="622"/>
+    <workbookView xWindow="120" yWindow="120" windowWidth="20835" windowHeight="12015" tabRatio="622" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Alle Abteilungen" sheetId="2" r:id="rId1"/>
@@ -498,9 +498,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -509,6 +506,9 @@
     </xf>
     <xf numFmtId="49" fontId="4" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="9" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -589,7 +589,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -1176,11 +1175,11 @@
         </c:dLbls>
         <c:gapWidth val="75"/>
         <c:overlap val="-25"/>
-        <c:axId val="107508480"/>
-        <c:axId val="107510016"/>
+        <c:axId val="105362560"/>
+        <c:axId val="105364096"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="107508480"/>
+        <c:axId val="105362560"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -1190,7 +1189,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="107510016"/>
+        <c:crossAx val="105364096"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1199,7 +1198,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="107510016"/>
+        <c:axId val="105364096"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="4"/>
@@ -1262,7 +1261,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="107508480"/>
+        <c:crossAx val="105362560"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="1"/>
@@ -1271,7 +1270,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -1612,11 +1610,11 @@
         </c:dLbls>
         <c:gapWidth val="75"/>
         <c:overlap val="-25"/>
-        <c:axId val="110541056"/>
-        <c:axId val="110542848"/>
+        <c:axId val="111796224"/>
+        <c:axId val="111797760"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="110541056"/>
+        <c:axId val="111796224"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -1626,7 +1624,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="110542848"/>
+        <c:crossAx val="111797760"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1635,7 +1633,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="110542848"/>
+        <c:axId val="111797760"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="4"/>
@@ -1698,7 +1696,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="110541056"/>
+        <c:crossAx val="111796224"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="1"/>
@@ -1751,7 +1749,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -1852,11 +1849,11 @@
         </c:dLbls>
         <c:gapWidth val="75"/>
         <c:overlap val="-25"/>
-        <c:axId val="110553344"/>
-        <c:axId val="110579712"/>
+        <c:axId val="104740736"/>
+        <c:axId val="104742272"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="110553344"/>
+        <c:axId val="104740736"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -1866,7 +1863,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="110579712"/>
+        <c:crossAx val="104742272"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1875,7 +1872,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="110579712"/>
+        <c:axId val="104742272"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="4"/>
@@ -1938,7 +1935,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="110553344"/>
+        <c:crossAx val="104740736"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="1"/>
@@ -1947,7 +1944,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -1997,7 +1993,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="1"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -2455,8 +2450,8 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="110637440"/>
-        <c:axId val="110639360"/>
+        <c:axId val="116518912"/>
+        <c:axId val="116520832"/>
       </c:barChart>
       <c:lineChart>
         <c:grouping val="stacked"/>
@@ -2573,11 +2568,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="110637440"/>
-        <c:axId val="110639360"/>
+        <c:axId val="116518912"/>
+        <c:axId val="116520832"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="110637440"/>
+        <c:axId val="116518912"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2586,7 +2581,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="110639360"/>
+        <c:crossAx val="116520832"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2594,7 +2589,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="110639360"/>
+        <c:axId val="116520832"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="4"/>
@@ -2774,7 +2769,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="110637440"/>
+        <c:crossAx val="116518912"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="1"/>
@@ -3216,11 +3211,11 @@
         </c:dLbls>
         <c:gapWidth val="75"/>
         <c:overlap val="-25"/>
-        <c:axId val="111220992"/>
-        <c:axId val="111235072"/>
+        <c:axId val="106825600"/>
+        <c:axId val="106827136"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="111220992"/>
+        <c:axId val="106825600"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -3230,7 +3225,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="111235072"/>
+        <c:crossAx val="106827136"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3239,7 +3234,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="111235072"/>
+        <c:axId val="106827136"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="4"/>
@@ -3302,7 +3297,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="111220992"/>
+        <c:crossAx val="106825600"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="1"/>
@@ -3355,7 +3350,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -3456,11 +3450,11 @@
         </c:dLbls>
         <c:gapWidth val="75"/>
         <c:overlap val="-25"/>
-        <c:axId val="111260032"/>
-        <c:axId val="111261568"/>
+        <c:axId val="106864640"/>
+        <c:axId val="106866176"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="111260032"/>
+        <c:axId val="106864640"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -3470,7 +3464,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="111261568"/>
+        <c:crossAx val="106866176"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3479,7 +3473,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="111261568"/>
+        <c:axId val="106866176"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="4"/>
@@ -3542,7 +3536,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="111260032"/>
+        <c:crossAx val="106864640"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="1"/>
@@ -3551,7 +3545,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -3598,7 +3591,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="1"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -4056,8 +4048,8 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="111044864"/>
-        <c:axId val="111063424"/>
+        <c:axId val="106915712"/>
+        <c:axId val="106938368"/>
       </c:barChart>
       <c:lineChart>
         <c:grouping val="stacked"/>
@@ -4174,11 +4166,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="111044864"/>
-        <c:axId val="111063424"/>
+        <c:axId val="106915712"/>
+        <c:axId val="106938368"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="111044864"/>
+        <c:axId val="106915712"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4187,7 +4179,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="111063424"/>
+        <c:crossAx val="106938368"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4195,7 +4187,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="111063424"/>
+        <c:axId val="106938368"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="4"/>
@@ -4375,7 +4367,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="111044864"/>
+        <c:crossAx val="106915712"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="1"/>
@@ -4790,11 +4782,11 @@
         </c:dLbls>
         <c:gapWidth val="75"/>
         <c:overlap val="-25"/>
-        <c:axId val="111161344"/>
-        <c:axId val="111162880"/>
+        <c:axId val="107011456"/>
+        <c:axId val="107017344"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="111161344"/>
+        <c:axId val="107011456"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -4804,7 +4796,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="111162880"/>
+        <c:crossAx val="107017344"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4813,7 +4805,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="111162880"/>
+        <c:axId val="107017344"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="4"/>
@@ -4876,7 +4868,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="111161344"/>
+        <c:crossAx val="107011456"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="1"/>
@@ -4929,7 +4921,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -5030,11 +5021,11 @@
         </c:dLbls>
         <c:gapWidth val="75"/>
         <c:overlap val="-25"/>
-        <c:axId val="111187840"/>
-        <c:axId val="111189376"/>
+        <c:axId val="111977984"/>
+        <c:axId val="111979520"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="111187840"/>
+        <c:axId val="111977984"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -5044,7 +5035,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="111189376"/>
+        <c:crossAx val="111979520"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -5053,7 +5044,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="111189376"/>
+        <c:axId val="111979520"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="4"/>
@@ -5116,7 +5107,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="111187840"/>
+        <c:crossAx val="111977984"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="1"/>
@@ -5125,7 +5116,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -5172,7 +5162,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="1"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -5630,8 +5619,8 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="111390720"/>
-        <c:axId val="111392640"/>
+        <c:axId val="116874624"/>
+        <c:axId val="116889088"/>
       </c:barChart>
       <c:lineChart>
         <c:grouping val="stacked"/>
@@ -5748,11 +5737,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="111390720"/>
-        <c:axId val="111392640"/>
+        <c:axId val="116874624"/>
+        <c:axId val="116889088"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="111390720"/>
+        <c:axId val="116874624"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5761,7 +5750,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="111392640"/>
+        <c:crossAx val="116889088"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -5769,7 +5758,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="111392640"/>
+        <c:axId val="116889088"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="4"/>
@@ -5949,7 +5938,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="111390720"/>
+        <c:crossAx val="116874624"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="1"/>
@@ -6312,11 +6301,11 @@
         </c:dLbls>
         <c:gapWidth val="75"/>
         <c:overlap val="-25"/>
-        <c:axId val="111436544"/>
-        <c:axId val="111438080"/>
+        <c:axId val="116609408"/>
+        <c:axId val="116610944"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="111436544"/>
+        <c:axId val="116609408"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -6326,7 +6315,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="111438080"/>
+        <c:crossAx val="116610944"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -6335,7 +6324,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="111438080"/>
+        <c:axId val="116610944"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="4"/>
@@ -6398,7 +6387,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="111436544"/>
+        <c:crossAx val="116609408"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="1"/>
@@ -6483,7 +6472,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -6584,11 +6572,11 @@
         </c:dLbls>
         <c:gapWidth val="75"/>
         <c:overlap val="-25"/>
-        <c:axId val="108137856"/>
-        <c:axId val="108168320"/>
+        <c:axId val="107057152"/>
+        <c:axId val="107058688"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="108137856"/>
+        <c:axId val="107057152"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -6598,7 +6586,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="108168320"/>
+        <c:crossAx val="107058688"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -6607,7 +6595,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="108168320"/>
+        <c:axId val="107058688"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="4"/>
@@ -6670,7 +6658,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="108137856"/>
+        <c:crossAx val="107057152"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="1"/>
@@ -6724,7 +6712,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -6825,11 +6812,11 @@
         </c:dLbls>
         <c:gapWidth val="75"/>
         <c:overlap val="-25"/>
-        <c:axId val="111463040"/>
-        <c:axId val="111473024"/>
+        <c:axId val="116627712"/>
+        <c:axId val="116645888"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="111463040"/>
+        <c:axId val="116627712"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -6839,7 +6826,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="111473024"/>
+        <c:crossAx val="116645888"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -6848,7 +6835,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="111473024"/>
+        <c:axId val="116645888"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="4"/>
@@ -6911,7 +6898,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="111463040"/>
+        <c:crossAx val="116627712"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="1"/>
@@ -6920,7 +6907,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -7441,8 +7427,8 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="108315392"/>
-        <c:axId val="108317312"/>
+        <c:axId val="116765056"/>
+        <c:axId val="116766976"/>
       </c:barChart>
       <c:lineChart>
         <c:grouping val="stacked"/>
@@ -7559,11 +7545,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="108315392"/>
-        <c:axId val="108317312"/>
+        <c:axId val="116765056"/>
+        <c:axId val="116766976"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="108315392"/>
+        <c:axId val="116765056"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7572,7 +7558,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="108317312"/>
+        <c:crossAx val="116766976"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -7580,7 +7566,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="108317312"/>
+        <c:axId val="116766976"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="4"/>
@@ -7760,7 +7746,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="108315392"/>
+        <c:crossAx val="116765056"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="1"/>
@@ -7838,7 +7824,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -8086,11 +8071,11 @@
         </c:dLbls>
         <c:gapWidth val="75"/>
         <c:overlap val="-25"/>
-        <c:axId val="112593536"/>
-        <c:axId val="112599424"/>
+        <c:axId val="117053696"/>
+        <c:axId val="117055488"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="112593536"/>
+        <c:axId val="117053696"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -8100,7 +8085,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="112599424"/>
+        <c:crossAx val="117055488"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -8109,7 +8094,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="112599424"/>
+        <c:axId val="117055488"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="4"/>
@@ -8172,7 +8157,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="112593536"/>
+        <c:crossAx val="117053696"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="1"/>
@@ -8181,7 +8166,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -8226,7 +8210,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -8327,11 +8310,11 @@
         </c:dLbls>
         <c:gapWidth val="75"/>
         <c:overlap val="-25"/>
-        <c:axId val="112640768"/>
-        <c:axId val="112642304"/>
+        <c:axId val="117072256"/>
+        <c:axId val="117073792"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="112640768"/>
+        <c:axId val="117072256"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -8341,7 +8324,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="112642304"/>
+        <c:crossAx val="117073792"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -8350,7 +8333,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="112642304"/>
+        <c:axId val="117073792"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="4"/>
@@ -8413,7 +8396,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="112640768"/>
+        <c:crossAx val="117072256"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="1"/>
@@ -8422,7 +8405,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -8940,8 +8922,8 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="95694208"/>
-        <c:axId val="95696384"/>
+        <c:axId val="117139712"/>
+        <c:axId val="117154176"/>
       </c:barChart>
       <c:lineChart>
         <c:grouping val="stacked"/>
@@ -9058,11 +9040,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="95694208"/>
-        <c:axId val="95696384"/>
+        <c:axId val="117139712"/>
+        <c:axId val="117154176"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="95694208"/>
+        <c:axId val="117139712"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9071,7 +9053,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="95696384"/>
+        <c:crossAx val="117154176"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -9079,7 +9061,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="95696384"/>
+        <c:axId val="117154176"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="4"/>
@@ -9259,7 +9241,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="95694208"/>
+        <c:crossAx val="117139712"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="1"/>
@@ -9331,7 +9313,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="1"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -9789,8 +9770,8 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="45923328"/>
-        <c:axId val="45937792"/>
+        <c:axId val="109970944"/>
+        <c:axId val="109972864"/>
       </c:barChart>
       <c:lineChart>
         <c:grouping val="stacked"/>
@@ -9907,11 +9888,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="45923328"/>
-        <c:axId val="45937792"/>
+        <c:axId val="109970944"/>
+        <c:axId val="109972864"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="45923328"/>
+        <c:axId val="109970944"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9920,7 +9901,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="45937792"/>
+        <c:crossAx val="109972864"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -9928,7 +9909,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="45937792"/>
+        <c:axId val="109972864"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="4"/>
@@ -10108,7 +10089,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="45923328"/>
+        <c:crossAx val="109970944"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="1"/>
@@ -10471,11 +10452,11 @@
         </c:dLbls>
         <c:gapWidth val="75"/>
         <c:overlap val="-25"/>
-        <c:axId val="108502016"/>
-        <c:axId val="108503808"/>
+        <c:axId val="110061824"/>
+        <c:axId val="110067712"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="108502016"/>
+        <c:axId val="110061824"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -10485,7 +10466,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="108503808"/>
+        <c:crossAx val="110067712"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -10494,7 +10475,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="108503808"/>
+        <c:axId val="110067712"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="4"/>
@@ -10557,7 +10538,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="108502016"/>
+        <c:crossAx val="110061824"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="1"/>
@@ -10610,7 +10591,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -10711,11 +10691,11 @@
         </c:dLbls>
         <c:gapWidth val="75"/>
         <c:overlap val="-25"/>
-        <c:axId val="108594304"/>
-        <c:axId val="108595840"/>
+        <c:axId val="110098304"/>
+        <c:axId val="110099840"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="108594304"/>
+        <c:axId val="110098304"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -10725,7 +10705,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="108595840"/>
+        <c:crossAx val="110099840"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -10734,7 +10714,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="108595840"/>
+        <c:axId val="110099840"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="4"/>
@@ -10797,7 +10777,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="108594304"/>
+        <c:crossAx val="110098304"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="1"/>
@@ -10806,7 +10786,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -10856,7 +10835,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="1"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -11314,8 +11292,8 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="108655360"/>
-        <c:axId val="108657280"/>
+        <c:axId val="111534464"/>
+        <c:axId val="111536384"/>
       </c:barChart>
       <c:lineChart>
         <c:grouping val="stacked"/>
@@ -11432,11 +11410,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="108655360"/>
-        <c:axId val="108657280"/>
+        <c:axId val="111534464"/>
+        <c:axId val="111536384"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="108655360"/>
+        <c:axId val="111534464"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -11445,7 +11423,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="108657280"/>
+        <c:crossAx val="111536384"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -11453,7 +11431,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="108657280"/>
+        <c:axId val="111536384"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="4"/>
@@ -11633,7 +11611,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="108655360"/>
+        <c:crossAx val="111534464"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="1"/>
@@ -11734,6 +11712,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -12077,11 +12056,11 @@
         </c:dLbls>
         <c:gapWidth val="75"/>
         <c:overlap val="-25"/>
-        <c:axId val="109041920"/>
-        <c:axId val="109047808"/>
+        <c:axId val="111599616"/>
+        <c:axId val="111601152"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="109041920"/>
+        <c:axId val="111599616"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -12091,7 +12070,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="109047808"/>
+        <c:crossAx val="111601152"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -12100,7 +12079,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="109047808"/>
+        <c:axId val="111601152"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="4"/>
@@ -12163,7 +12142,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="109041920"/>
+        <c:crossAx val="111599616"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="1"/>
@@ -12172,6 +12151,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -12317,11 +12297,11 @@
         </c:dLbls>
         <c:gapWidth val="75"/>
         <c:overlap val="-25"/>
-        <c:axId val="109080576"/>
-        <c:axId val="109082112"/>
+        <c:axId val="111622016"/>
+        <c:axId val="111623552"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="109080576"/>
+        <c:axId val="111622016"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -12331,7 +12311,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="109082112"/>
+        <c:crossAx val="111623552"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -12340,7 +12320,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="109082112"/>
+        <c:axId val="111623552"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="4"/>
@@ -12403,7 +12383,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="109080576"/>
+        <c:crossAx val="111622016"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="1"/>
@@ -12917,8 +12897,8 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="109143936"/>
-        <c:axId val="109150208"/>
+        <c:axId val="116481408"/>
+        <c:axId val="116487680"/>
       </c:barChart>
       <c:lineChart>
         <c:grouping val="stacked"/>
@@ -13035,11 +13015,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="109143936"/>
-        <c:axId val="109150208"/>
+        <c:axId val="116481408"/>
+        <c:axId val="116487680"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="109143936"/>
+        <c:axId val="116481408"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -13048,7 +13028,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="109150208"/>
+        <c:crossAx val="116487680"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -13056,7 +13036,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="109150208"/>
+        <c:axId val="116487680"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="4"/>
@@ -13235,7 +13215,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="109143936"/>
+        <c:crossAx val="116481408"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="1"/>
@@ -14367,8 +14347,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:ID72"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B16" workbookViewId="0">
-      <selection activeCell="S53" sqref="S53"/>
+    <sheetView topLeftCell="M1" workbookViewId="0">
+      <selection activeCell="M22" sqref="M22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -14712,7 +14692,7 @@
         <f>SUM(W12:W14)</f>
         <v>37</v>
       </c>
-      <c r="AJ15" s="39" t="s">
+      <c r="AJ15" s="38" t="s">
         <v>64</v>
       </c>
     </row>
@@ -14804,7 +14784,7 @@
       <c r="AH17" s="29" t="s">
         <v>53</v>
       </c>
-      <c r="AJ17" s="38" t="s">
+      <c r="AJ17" s="37" t="s">
         <v>21</v>
       </c>
       <c r="AK17" s="10" t="s">
@@ -14879,7 +14859,7 @@
       <c r="BH17" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="BI17" s="38" t="s">
+      <c r="BI17" s="37" t="s">
         <v>20</v>
       </c>
       <c r="BJ17" s="10" t="s">
@@ -14948,7 +14928,7 @@
       <c r="CE17" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="CF17" s="38" t="s">
+      <c r="CF17" s="37" t="s">
         <v>20</v>
       </c>
       <c r="CG17" s="10" t="s">
@@ -15011,7 +14991,7 @@
       <c r="CZ17" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="DA17" s="38" t="s">
+      <c r="DA17" s="37" t="s">
         <v>20</v>
       </c>
       <c r="DB17" s="10" t="s">
@@ -15098,7 +15078,7 @@
       <c r="EC17" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="ED17" s="38" t="s">
+      <c r="ED17" s="37" t="s">
         <v>20</v>
       </c>
       <c r="EE17" s="10" t="s">
@@ -15242,7 +15222,7 @@
       <c r="FY17" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="FZ17" s="38" t="s">
+      <c r="FZ17" s="37" t="s">
         <v>20</v>
       </c>
       <c r="GA17" s="10" t="s">
@@ -15302,7 +15282,7 @@
       <c r="GS17" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="GT17" s="38" t="s">
+      <c r="GT17" s="37" t="s">
         <v>20</v>
       </c>
       <c r="GU17" s="10" t="s">
@@ -15484,7 +15464,7 @@
         <v>0.97499999999999998</v>
       </c>
       <c r="AH18" s="8">
-        <f t="shared" ref="AF18:AH18" si="0">AD18-AC18</f>
+        <f t="shared" ref="AH18" si="0">AD18-AC18</f>
         <v>1</v>
       </c>
       <c r="AJ18" s="24">
@@ -16840,7 +16820,7 @@
         <v>4</v>
       </c>
       <c r="AE20" s="8">
-        <f t="shared" ref="AE19:AE25" si="7">AA20-Z20</f>
+        <f t="shared" ref="AE20:AE25" si="7">AA20-Z20</f>
         <v>1</v>
       </c>
       <c r="AF20" s="8">
@@ -17502,7 +17482,7 @@
         <v>0.97499999999999998</v>
       </c>
       <c r="AH21" s="8">
-        <f t="shared" ref="AH19:AH25" si="8">AD21-AC21</f>
+        <f t="shared" ref="AH21:AH24" si="8">AD21-AC21</f>
         <v>1</v>
       </c>
       <c r="AJ21" s="24">
@@ -19521,7 +19501,7 @@
         <v>0.95</v>
       </c>
       <c r="AG24" s="8">
-        <f t="shared" ref="AG19:AG25" si="9">AC24-AB24</f>
+        <f t="shared" ref="AG24" si="9">AC24-AB24</f>
         <v>1</v>
       </c>
       <c r="AH24" s="8">
@@ -20133,7 +20113,7 @@
       </c>
     </row>
     <row r="25" spans="1:238" x14ac:dyDescent="0.25">
-      <c r="A25" s="36" t="s">
+      <c r="A25" s="35" t="s">
         <v>63</v>
       </c>
       <c r="D25">
@@ -20197,7 +20177,7 @@
         <v>1</v>
       </c>
       <c r="AF25" s="8">
-        <f t="shared" ref="AF19:AF25" si="10">AB25-AA25</f>
+        <f t="shared" ref="AF25" si="10">AB25-AA25</f>
         <v>1</v>
       </c>
       <c r="AG25" s="8">
@@ -20817,7 +20797,7 @@
       </c>
     </row>
     <row r="26" spans="1:238" x14ac:dyDescent="0.25">
-      <c r="A26" s="37"/>
+      <c r="A26" s="36"/>
     </row>
     <row r="27" spans="1:238" x14ac:dyDescent="0.25">
       <c r="A27" s="3"/>
@@ -20963,7 +20943,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AM45"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="AB13" workbookViewId="0">
       <selection activeCell="B3" sqref="B3:Z11"/>
     </sheetView>
   </sheetViews>
@@ -23365,7 +23345,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AK45"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="AD17" workbookViewId="0">
       <selection activeCell="X11" sqref="B3:X11"/>
     </sheetView>
   </sheetViews>
@@ -24499,34 +24479,34 @@
         <v>Kommentare der Befragten:
 (schriftlich oder mündlich)</v>
       </c>
-      <c r="B13" s="35" t="s">
+      <c r="B13" s="39" t="s">
         <v>44</v>
       </c>
-      <c r="C13" s="35"/>
-      <c r="D13" s="35"/>
-      <c r="E13" s="35"/>
-      <c r="F13" s="35"/>
-      <c r="G13" s="35"/>
-      <c r="H13" s="35"/>
-      <c r="I13" s="35"/>
-      <c r="J13" s="35"/>
-      <c r="K13" s="35"/>
-      <c r="L13" s="35"/>
-      <c r="M13" s="35"/>
-      <c r="N13" s="35"/>
-      <c r="O13" s="35"/>
-      <c r="P13" s="35"/>
-      <c r="Q13" s="35"/>
-      <c r="R13" s="35"/>
-      <c r="S13" s="35"/>
-      <c r="T13" s="35"/>
-      <c r="U13" s="35"/>
-      <c r="V13" s="35"/>
-      <c r="W13" s="35"/>
-      <c r="X13" s="35"/>
-      <c r="Y13" s="35"/>
-      <c r="Z13" s="35"/>
-      <c r="AA13" s="35"/>
+      <c r="C13" s="39"/>
+      <c r="D13" s="39"/>
+      <c r="E13" s="39"/>
+      <c r="F13" s="39"/>
+      <c r="G13" s="39"/>
+      <c r="H13" s="39"/>
+      <c r="I13" s="39"/>
+      <c r="J13" s="39"/>
+      <c r="K13" s="39"/>
+      <c r="L13" s="39"/>
+      <c r="M13" s="39"/>
+      <c r="N13" s="39"/>
+      <c r="O13" s="39"/>
+      <c r="P13" s="39"/>
+      <c r="Q13" s="39"/>
+      <c r="R13" s="39"/>
+      <c r="S13" s="39"/>
+      <c r="T13" s="39"/>
+      <c r="U13" s="39"/>
+      <c r="V13" s="39"/>
+      <c r="W13" s="39"/>
+      <c r="X13" s="39"/>
+      <c r="Y13" s="39"/>
+      <c r="Z13" s="39"/>
+      <c r="AA13" s="39"/>
       <c r="AB13" s="28"/>
       <c r="AC13" s="28"/>
       <c r="AD13" s="28"/>
@@ -24538,34 +24518,34 @@
     </row>
     <row r="14" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A14" s="19"/>
-      <c r="B14" s="35" t="s">
+      <c r="B14" s="39" t="s">
         <v>45</v>
       </c>
-      <c r="C14" s="35"/>
-      <c r="D14" s="35"/>
-      <c r="E14" s="35"/>
-      <c r="F14" s="35"/>
-      <c r="G14" s="35"/>
-      <c r="H14" s="35"/>
-      <c r="I14" s="35"/>
-      <c r="J14" s="35"/>
-      <c r="K14" s="35"/>
-      <c r="L14" s="35"/>
-      <c r="M14" s="35"/>
-      <c r="N14" s="35"/>
-      <c r="O14" s="35"/>
-      <c r="P14" s="35"/>
-      <c r="Q14" s="35"/>
-      <c r="R14" s="35"/>
-      <c r="S14" s="35"/>
-      <c r="T14" s="35"/>
-      <c r="U14" s="35"/>
-      <c r="V14" s="35"/>
-      <c r="W14" s="35"/>
-      <c r="X14" s="35"/>
-      <c r="Y14" s="35"/>
-      <c r="Z14" s="35"/>
-      <c r="AA14" s="35"/>
+      <c r="C14" s="39"/>
+      <c r="D14" s="39"/>
+      <c r="E14" s="39"/>
+      <c r="F14" s="39"/>
+      <c r="G14" s="39"/>
+      <c r="H14" s="39"/>
+      <c r="I14" s="39"/>
+      <c r="J14" s="39"/>
+      <c r="K14" s="39"/>
+      <c r="L14" s="39"/>
+      <c r="M14" s="39"/>
+      <c r="N14" s="39"/>
+      <c r="O14" s="39"/>
+      <c r="P14" s="39"/>
+      <c r="Q14" s="39"/>
+      <c r="R14" s="39"/>
+      <c r="S14" s="39"/>
+      <c r="T14" s="39"/>
+      <c r="U14" s="39"/>
+      <c r="V14" s="39"/>
+      <c r="W14" s="39"/>
+      <c r="X14" s="39"/>
+      <c r="Y14" s="39"/>
+      <c r="Z14" s="39"/>
+      <c r="AA14" s="39"/>
       <c r="AB14" s="28"/>
       <c r="AC14" s="28"/>
       <c r="AD14" s="28"/>
@@ -25965,7 +25945,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AI35"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="AB13" workbookViewId="0">
       <selection activeCell="B3" sqref="B3:V11"/>
     </sheetView>
   </sheetViews>
@@ -32829,59 +32809,59 @@
         <v>Kommentare der Befragten:
 (schriftlich oder mündlich)</v>
       </c>
-      <c r="B13" s="35" t="s">
+      <c r="B13" s="39" t="s">
         <v>46</v>
       </c>
-      <c r="C13" s="35"/>
-      <c r="D13" s="35"/>
-      <c r="E13" s="35"/>
-      <c r="F13" s="35"/>
-      <c r="G13" s="35"/>
-      <c r="H13" s="35"/>
-      <c r="I13" s="35"/>
-      <c r="J13" s="35"/>
-      <c r="K13" s="35"/>
-      <c r="L13" s="35"/>
-      <c r="M13" s="35"/>
-      <c r="N13" s="35"/>
-      <c r="O13" s="35"/>
-      <c r="P13" s="35"/>
-      <c r="Q13" s="35"/>
-      <c r="R13" s="35"/>
-      <c r="S13" s="35"/>
-      <c r="T13" s="35"/>
-      <c r="U13" s="35"/>
-      <c r="V13" s="35"/>
-      <c r="W13" s="35"/>
-      <c r="X13" s="35"/>
-      <c r="Y13" s="35"/>
-      <c r="Z13" s="35"/>
-      <c r="AA13" s="35"/>
-      <c r="AB13" s="35"/>
-      <c r="AC13" s="35"/>
-      <c r="AD13" s="35"/>
-      <c r="AE13" s="35"/>
-      <c r="AF13" s="35"/>
-      <c r="AG13" s="35"/>
-      <c r="AH13" s="35"/>
-      <c r="AI13" s="35"/>
-      <c r="AJ13" s="35"/>
-      <c r="AK13" s="35"/>
-      <c r="AL13" s="35"/>
-      <c r="AM13" s="35"/>
-      <c r="AN13" s="35"/>
-      <c r="AO13" s="35"/>
-      <c r="AP13" s="35"/>
-      <c r="AQ13" s="35"/>
-      <c r="AR13" s="35"/>
-      <c r="AS13" s="35"/>
-      <c r="AT13" s="35"/>
-      <c r="AU13" s="35"/>
-      <c r="AV13" s="35"/>
-      <c r="AW13" s="35"/>
-      <c r="AX13" s="35"/>
-      <c r="AY13" s="35"/>
-      <c r="AZ13" s="35"/>
+      <c r="C13" s="39"/>
+      <c r="D13" s="39"/>
+      <c r="E13" s="39"/>
+      <c r="F13" s="39"/>
+      <c r="G13" s="39"/>
+      <c r="H13" s="39"/>
+      <c r="I13" s="39"/>
+      <c r="J13" s="39"/>
+      <c r="K13" s="39"/>
+      <c r="L13" s="39"/>
+      <c r="M13" s="39"/>
+      <c r="N13" s="39"/>
+      <c r="O13" s="39"/>
+      <c r="P13" s="39"/>
+      <c r="Q13" s="39"/>
+      <c r="R13" s="39"/>
+      <c r="S13" s="39"/>
+      <c r="T13" s="39"/>
+      <c r="U13" s="39"/>
+      <c r="V13" s="39"/>
+      <c r="W13" s="39"/>
+      <c r="X13" s="39"/>
+      <c r="Y13" s="39"/>
+      <c r="Z13" s="39"/>
+      <c r="AA13" s="39"/>
+      <c r="AB13" s="39"/>
+      <c r="AC13" s="39"/>
+      <c r="AD13" s="39"/>
+      <c r="AE13" s="39"/>
+      <c r="AF13" s="39"/>
+      <c r="AG13" s="39"/>
+      <c r="AH13" s="39"/>
+      <c r="AI13" s="39"/>
+      <c r="AJ13" s="39"/>
+      <c r="AK13" s="39"/>
+      <c r="AL13" s="39"/>
+      <c r="AM13" s="39"/>
+      <c r="AN13" s="39"/>
+      <c r="AO13" s="39"/>
+      <c r="AP13" s="39"/>
+      <c r="AQ13" s="39"/>
+      <c r="AR13" s="39"/>
+      <c r="AS13" s="39"/>
+      <c r="AT13" s="39"/>
+      <c r="AU13" s="39"/>
+      <c r="AV13" s="39"/>
+      <c r="AW13" s="39"/>
+      <c r="AX13" s="39"/>
+      <c r="AY13" s="39"/>
+      <c r="AZ13" s="39"/>
     </row>
     <row r="14" spans="1:61" x14ac:dyDescent="0.25">
       <c r="A14" s="4"/>
@@ -35475,11 +35455,11 @@
         <v>4</v>
       </c>
       <c r="AD7" s="8">
-        <f t="shared" ref="AD6:AD9" si="11">Z7-Y7</f>
+        <f t="shared" ref="AD7:AD9" si="11">Z7-Y7</f>
         <v>1</v>
       </c>
       <c r="AE7" s="8">
-        <f t="shared" ref="AE5:AE9" si="12">AA7-Z7</f>
+        <f t="shared" ref="AE7:AE9" si="12">AA7-Z7</f>
         <v>0.5</v>
       </c>
       <c r="AF7" s="8">
@@ -37498,7 +37478,7 @@
         <v>0.9</v>
       </c>
       <c r="AX5" s="8">
-        <f t="shared" ref="AX5:AX11" si="9">AT5-AS5</f>
+        <f t="shared" ref="AX5:AX10" si="9">AT5-AS5</f>
         <v>2</v>
       </c>
     </row>
@@ -37648,11 +37628,11 @@
         <v>4</v>
       </c>
       <c r="AU6" s="8">
-        <f t="shared" ref="AU5:AU11" si="10">AQ6-AP6</f>
+        <f t="shared" ref="AU6:AU11" si="10">AQ6-AP6</f>
         <v>1</v>
       </c>
       <c r="AV6" s="8">
-        <f t="shared" ref="AV5:AV11" si="11">AR6-AQ6</f>
+        <f t="shared" ref="AV6:AV10" si="11">AR6-AQ6</f>
         <v>1</v>
       </c>
       <c r="AW6" s="8">
@@ -38131,7 +38111,7 @@
         <v>1</v>
       </c>
       <c r="AW9" s="8">
-        <f t="shared" ref="AW5:AW11" si="12">AS9-AR9</f>
+        <f t="shared" ref="AW9:AW10" si="12">AS9-AR9</f>
         <v>0.25</v>
       </c>
       <c r="AX9" s="8">

</xml_diff>